<commit_message>
Lys Gia Huy _B25DTCN099_sesssion12_btvn
</commit_message>
<xml_diff>
--- a/btvn/BTVN5.xlsx
+++ b/btvn/BTVN5.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,43 +24,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Họ tên</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Môn học</t>
+  </si>
+  <si>
+    <t>Điểm 1</t>
+  </si>
+  <si>
+    <t>Điểm 2</t>
+  </si>
+  <si>
+    <t>Điểm 3</t>
   </si>
   <si>
     <t>Toán</t>
   </si>
   <si>
-    <t>Văn</t>
-  </si>
-  <si>
-    <t>Anh</t>
-  </si>
-  <si>
-    <t>Tổng điểm</t>
-  </si>
-  <si>
-    <t>Nguyễn An</t>
-  </si>
-  <si>
-    <t>Lê Bình</t>
-  </si>
-  <si>
-    <t>Trần Cường</t>
-  </si>
-  <si>
-    <t>Phạm Dung</t>
+    <t>Tin học</t>
+  </si>
+  <si>
+    <t>Tiếng Anh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng điểm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">điểm trung bình </t>
+  </si>
+  <si>
+    <t>Điểm cao nhất</t>
+  </si>
+  <si>
+    <t>điểm thấp nhất</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,15 +73,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="SFProDisplay"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="SFProDisplay"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,10 +102,36 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -107,13 +140,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -395,116 +431,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:I8"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="4:9" ht="31.5">
-      <c r="D4" s="1" t="s">
+    <row r="1" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="B2" s="2">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <f>MAX(B2:D2)</f>
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f>MIN(B2:D2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="0">SUM(B3:D3)</f>
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F4" si="1">AVERAGE(B3:D3)</f>
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G4" si="2">MAX(B3:D3)</f>
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="3">MIN(B3:D3)</f>
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="4:9" ht="30">
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
+    <row r="4" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="B4" s="2">
         <v>6</v>
       </c>
-      <c r="I5" s="2">
-        <f>SUM(F5:H5)</f>
+      <c r="C4" s="2">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="4:9" ht="15">
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
         <v>6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>8</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" ref="I6:I8" si="0">SUM(F6:H6)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="4:9" ht="30">
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2">
-        <v>7</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" ht="30">
-      <c r="D8" s="2">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2">
-        <v>8</v>
-      </c>
-      <c r="H8" s="2">
-        <v>9</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="0"/>
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>